<commit_message>
may làm duoc trung oi
</commit_message>
<xml_diff>
--- a/10_Management/Exam_PMP_Finish_07032019 - TrungLV_Final.xlsx
+++ b/10_Management/Exam_PMP_Finish_07032019 - TrungLV_Final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\EBill\10_Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Working\EBill\10_Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76A0806-10EC-4041-ACA7-3ED85B8CC00F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D91454-BA99-4E62-9BD5-B4F96DC3F735}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{957D22A2-4D54-4148-9DDE-7A2AF7FA87D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="11" xr2:uid="{957D22A2-4D54-4148-9DDE-7A2AF7FA87D7}"/>
   </bookViews>
   <sheets>
     <sheet name="study plan" sheetId="59" r:id="rId1"/>
@@ -67,7 +67,8 @@
     <sheet name="Monitoring" sheetId="5" r:id="rId52"/>
     <sheet name="Closing" sheetId="6" r:id="rId53"/>
     <sheet name="Mock" sheetId="8" r:id="rId54"/>
-    <sheet name="Full Test 4" sheetId="9" r:id="rId55"/>
+    <sheet name="Full test 1" sheetId="61" r:id="rId55"/>
+    <sheet name="Full Test 4" sheetId="9" r:id="rId56"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -108,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2240" uniqueCount="1141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2389" uniqueCount="1208">
   <si>
     <t>No</t>
   </si>
@@ -3707,12 +3708,221 @@
   <si>
     <t>Việc dành nhiều money and managing resource nên đang ở execution phase of the project. Hence stakeholder influence is now less than in previous phase</t>
   </si>
+  <si>
+    <t>Thằng PM có nhiều quyền không chỉ . Identify, monitor, and respond to risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Choice 3. Carry out performance appraisal of project team: thực hiện đánh giá hiệu suất của nhóm dự án thì trong function tổ chức PM k có quyền đó</t>
+  </si>
+  <si>
+    <t>Hỏi thầy</t>
+  </si>
+  <si>
+    <t>việc make -or buy analysis thì vẫn phải tuân theo core business của tổ chức</t>
+  </si>
+  <si>
+    <t>Xem lý thuyết của wbs diction: description of work, responsible organization, and schedule milestones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sắp xong dự án thì các team member thay vì làm nhiệm vụ của họ thì tìm một vị trí mới đấy là safety </t>
+  </si>
+  <si>
+    <t>trc đây làm cho cty A, giờ chuyển sang làm cho công ty đối thủ thì vẫn You can use the knowledge gained in the first company to improve your present company`s product quality</t>
+  </si>
+  <si>
+    <t>you had not anticipated earlier. Key word: do chưa xác định được nên cần phải tiến hành analysis, Perform updated risk identification and analysis</t>
+  </si>
+  <si>
+    <t>you wish to manage procurement relationships, monitor contract performance, and make changes and corrections as needed =&gt; là nằm trong process control procurment và cần xác định input/output của process này là gì</t>
+  </si>
+  <si>
+    <t>Trong control procurment thì  Project schedule không là input</t>
+  </si>
+  <si>
+    <t>Xem xét crashing cần đánh giá cả tổng time saving và cost crash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">collect work performance là một phần trong direct and manage </t>
+  </si>
+  <si>
+    <t>Thuyết X là nói về vấn đề: To get the work done, the supervisor threatens punishment and strictly supervises the work</t>
+  </si>
+  <si>
+    <t>MỤc tiêu của dự án không phải là mục tiêu của dự án trước đấy được with the goals of previous projects</t>
+  </si>
+  <si>
+    <t>you are currently involved in monitoring stakeholder relationships and adjusting plans for their engagement thì là control process stakeholder</t>
+  </si>
+  <si>
+    <t>Cần phải relax</t>
+  </si>
+  <si>
+    <t>Control chart mới có set limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> you have documents to highlight project status, lessons learned, issue logs, and outputs from other knowledge areas =&gt; document inlcude trong Project communications</t>
+  </si>
+  <si>
+    <t>which of the following is NOT the responsibility of both the project sponsor and the customer không liên quan tới Provide financial resources for the project</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hybrid type of contractual arrangement là hợp đồng time and material contracts</t>
+  </si>
+  <si>
+    <t>pre-defined budget là constraint</t>
+  </si>
+  <si>
+    <t>When does the project manager review prior phase documentation and customer acceptance documentation from the Validate Scope process? =&gt; Close Project or Phase</t>
+  </si>
+  <si>
+    <t>Management Style: directing: cầm tay chỉ việc
+Coaching: huấn luyện
+Supporting: hỗ trợ
+Delegating: ủy quyền, trao quyền
+Cần phải hiểu: tell them when and how the tasks should be completed là direct</t>
+  </si>
+  <si>
+    <t>Sau khi ranking ra rồi, phân loại ra rồi lại tiếp tục đưa ra để phân tích sâu thêm: Analyze the effect of identified risks on overall project objectives</t>
+  </si>
+  <si>
+    <t>Mean  = (P+O + 4M)/6; six sigma = Mean +-6 = 13-6*1=7 và 13 + 6*1 = 19</t>
+  </si>
+  <si>
+    <t>Lesson learn: At the end of a project or phase, the information is transferred to an organizational process asset called a Lessons learned repository.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Update Organizational Process Assets là throuough project còn  Update Organizational Process Assets là Create project closure documents</t>
+  </si>
+  <si>
+    <t>Stakeholder analysis is used to systematically gather and analyze quantitative and qualitative information on stakeholders' level of interest in the project. In this technique: =&gt; Stakeholders are identified based on degree of interest</t>
+  </si>
+  <si>
+    <t>Warranty costs là chi phí phát sinh bên ngoài nên not incurred toward ensuring compliance to requirements?</t>
+  </si>
+  <si>
+    <t>Vấn đề đang nói you are in the process of determining the project roles, responsibilities, and reporting relationships for your team members là nằm trong process resource management plan còn Project team assignments output của acquairesource</t>
+  </si>
+  <si>
+    <t>cope statement provides  Common understanding of the project scope among project stakeholders.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  following statements on quality planning </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Team members are scared and disappointed as they learn they will be out of a project =&gt; ủy quyền cho HR</t>
+  </si>
+  <si>
+    <t>team use these scripts to test the modules and in what process would the test scripts be audited to ensure they are valid =&gt; Control Quality, Manage Quality</t>
+  </si>
+  <si>
+    <t>Quản lý kỳ vọng của stakeholder là PM</t>
+  </si>
+  <si>
+    <t>Using the DfX may result in mục đích là để giảm chi phí reduce cost chứ không phải quality</t>
+  </si>
+  <si>
+    <t>Chane control tool trong Perform Integrated Change Control process bao gồm: configuration identification, status accounting, verification and audit</t>
+  </si>
+  <si>
+    <t>Không hiểu hỏi thầy</t>
+  </si>
+  <si>
+    <t>In the last project status meeting, a team member criticized some of his teammates and undermined the status of work done by them. The role that was played by the person was that of: Aggressor</t>
+  </si>
+  <si>
+    <t>Đọc lại mục này</t>
+  </si>
+  <si>
+    <t>MOST LIKELY reason for the variances in the project schedule and budget? Là Assumptions used in the planning processes were not valid</t>
+  </si>
+  <si>
+    <t>Đọc kỹ câu hỏi, nếu task A,B,C là critical thì mới xác định dc critical path</t>
+  </si>
+  <si>
+    <t>Cần hiểu câu hỏi là khi mà đang làm với tài liệu nào, planning stakeholder thì cần phải follow tài liệu nào từ process  Identify Stakeholders</t>
+  </si>
+  <si>
+    <t>Khi tạo managemeng sig zigma -&gt; cost management plan for your Six-Sigma project =&gt;Uses preferred tools for cost estimating</t>
+  </si>
+  <si>
+    <t>determining the project roles, responsibilities and reporting relationships for your team members nằm trong plan resource management</t>
+  </si>
+  <si>
+    <t>Audit chỉ trong manage quality</t>
+  </si>
+  <si>
+    <t>, these guidelines and policies will be classified là constraints</t>
+  </si>
+  <si>
+    <t>Identify Stakeholders is the process of identifying all people or organizations impacted by the project and to document: Stakeholder interests, involvement, and impact on project success</t>
+  </si>
+  <si>
+    <t>Which of the following exhibits greatest resistance to change =&gt; people</t>
+  </si>
+  <si>
+    <t>The closure of a phase is required to be approved in some form before it can be considered closed. Là characteristic of a project phase. Vì các quy trình của dự án có thể gộp lại với nhau</t>
+  </si>
+  <si>
+    <t>Develop Schedule process sử dụng tool technique là simulation</t>
+  </si>
+  <si>
+    <t>The activity list should include descriptions of activities. Activity liên quan tới team member Ensure that the team members understand what work is to be completed</t>
+  </si>
+  <si>
+    <t>EMV = total probbility * total impact cái nào lớn thì concern lớn nhất</t>
+  </si>
+  <si>
+    <t>output của Plan Scope Management process là Scope management plan and Requirements management plan</t>
+  </si>
+  <si>
+    <t>Control Quality is the process of monitoring and recording results of executing the quality activities: Sampling and probability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data analysis techniques trong Plan Cost Management process  Reviewing strategic funding such as: self-funding, funding with equity, or funding with debt </t>
+  </si>
+  <si>
+    <t>Các bài dưới 60%</t>
+  </si>
+  <si>
+    <t>Trạng thái review</t>
+  </si>
+  <si>
+    <t>Planning 6</t>
+  </si>
+  <si>
+    <t>Monitoring 1</t>
+  </si>
+  <si>
+    <t>Monitoring 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Monitoring 5</t>
+  </si>
+  <si>
+    <t>Executing 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Mock Exam 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Mock Exam 17</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
+    <t>Procurement</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3857,8 +4067,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3934,6 +4150,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4287,7 +4515,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4575,6 +4803,21 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="13" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="17" fillId="13" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="13" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="13" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -4597,21 +4840,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="13" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="17" fillId="13" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="13" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4629,86 +4868,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Callout: Line with Border and Accent Bar 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5B5370C-BB2A-469E-BB6A-648ED9D610B4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10496550" y="4772024"/>
-          <a:ext cx="2924175" cy="962026"/>
-        </a:xfrm>
-        <a:prstGeom prst="accentBorderCallout1">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Cần</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> dừng lại để review trong tuần này bao gồm:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>+ Kiến thức + các bài tập</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5013,8 +5172,8 @@
   </sheetPr>
   <dimension ref="A1:AA1017"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView topLeftCell="E23" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -5022,7 +5181,9 @@
     <col min="1" max="1" width="26.28515625" style="101" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="14.42578125" style="101"/>
     <col min="6" max="9" width="14.42578125" style="47"/>
-    <col min="10" max="16384" width="14.42578125" style="101"/>
+    <col min="10" max="10" width="30.140625" style="101" customWidth="1"/>
+    <col min="11" max="11" width="20" style="101" customWidth="1"/>
+    <col min="12" max="16384" width="14.42578125" style="101"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15">
@@ -5053,8 +5214,12 @@
       <c r="I1" s="50" t="s">
         <v>540</v>
       </c>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
+      <c r="J1" s="47" t="s">
+        <v>1197</v>
+      </c>
+      <c r="K1" s="47" t="s">
+        <v>1198</v>
+      </c>
       <c r="L1" s="47"/>
       <c r="M1" s="47"/>
       <c r="N1" s="47"/>
@@ -5092,7 +5257,9 @@
       <c r="I2" s="50" t="s">
         <v>540</v>
       </c>
-      <c r="J2" s="47"/>
+      <c r="J2" s="47" t="s">
+        <v>489</v>
+      </c>
       <c r="K2" s="47"/>
       <c r="L2" s="47"/>
       <c r="M2" s="47"/>
@@ -5131,7 +5298,9 @@
       <c r="I3" s="50" t="s">
         <v>540</v>
       </c>
-      <c r="J3" s="47"/>
+      <c r="J3" s="47" t="s">
+        <v>488</v>
+      </c>
       <c r="K3" s="47"/>
       <c r="L3" s="47"/>
       <c r="M3" s="47"/>
@@ -5170,7 +5339,9 @@
       <c r="I4" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J4" s="47"/>
+      <c r="J4" s="47" t="s">
+        <v>486</v>
+      </c>
       <c r="K4" s="47"/>
       <c r="L4" s="47"/>
       <c r="M4" s="47"/>
@@ -5209,7 +5380,9 @@
       <c r="I5" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J5" s="47"/>
+      <c r="J5" s="47" t="s">
+        <v>484</v>
+      </c>
       <c r="K5" s="47"/>
       <c r="L5" s="47"/>
       <c r="M5" s="47"/>
@@ -5254,7 +5427,9 @@
       <c r="I6" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J6" s="47"/>
+      <c r="J6" s="116" t="s">
+        <v>1199</v>
+      </c>
       <c r="K6" s="47"/>
       <c r="L6" s="47"/>
       <c r="M6" s="47"/>
@@ -5293,7 +5468,9 @@
       <c r="I7" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J7" s="47"/>
+      <c r="J7" s="47" t="s">
+        <v>1200</v>
+      </c>
       <c r="K7" s="47"/>
       <c r="L7" s="47"/>
       <c r="M7" s="47"/>
@@ -5338,7 +5515,9 @@
       <c r="I8" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J8" s="47"/>
+      <c r="J8" s="47" t="s">
+        <v>482</v>
+      </c>
       <c r="K8" s="47"/>
       <c r="L8" s="47"/>
       <c r="M8" s="47"/>
@@ -5383,7 +5562,9 @@
       <c r="I9" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J9" s="47"/>
+      <c r="J9" s="47" t="s">
+        <v>481</v>
+      </c>
       <c r="K9" s="47"/>
       <c r="L9" s="47"/>
       <c r="M9" s="47"/>
@@ -5428,7 +5609,9 @@
       <c r="I10" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J10" s="47"/>
+      <c r="J10" s="47" t="s">
+        <v>1201</v>
+      </c>
       <c r="K10" s="47"/>
       <c r="L10" s="47"/>
       <c r="M10" s="47"/>
@@ -5447,7 +5630,7 @@
       <c r="Z10" s="47"/>
       <c r="AA10" s="47"/>
     </row>
-    <row r="11" spans="1:27" ht="15">
+    <row r="11" spans="1:27" ht="25.5">
       <c r="A11" s="61" t="s">
         <v>352</v>
       </c>
@@ -5473,7 +5656,9 @@
       <c r="I11" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J11" s="47"/>
+      <c r="J11" s="120" t="s">
+        <v>1202</v>
+      </c>
       <c r="K11" s="47"/>
       <c r="L11" s="47"/>
       <c r="M11" s="47"/>
@@ -5516,7 +5701,9 @@
         <v>386</v>
       </c>
       <c r="I12" s="50"/>
-      <c r="J12" s="47"/>
+      <c r="J12" s="121" t="s">
+        <v>480</v>
+      </c>
       <c r="K12" s="47"/>
       <c r="L12" s="47"/>
       <c r="M12" s="47"/>
@@ -5560,7 +5747,9 @@
       <c r="I13" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J13" s="47"/>
+      <c r="J13" s="121" t="s">
+        <v>478</v>
+      </c>
       <c r="K13" s="47"/>
       <c r="L13" s="47"/>
       <c r="M13" s="47"/>
@@ -5604,7 +5793,9 @@
       <c r="I14" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J14" s="47"/>
+      <c r="J14" s="121" t="s">
+        <v>477</v>
+      </c>
       <c r="K14" s="47"/>
       <c r="L14" s="47"/>
       <c r="M14" s="47"/>
@@ -5627,10 +5818,10 @@
       <c r="A15" s="62" t="s">
         <v>369</v>
       </c>
-      <c r="B15" s="103">
+      <c r="B15" s="108">
         <v>43473</v>
       </c>
-      <c r="C15" s="103" t="str">
+      <c r="C15" s="108" t="str">
         <f t="shared" si="1"/>
         <v>Thứ 3</v>
       </c>
@@ -5648,7 +5839,9 @@
       <c r="I15" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J15" s="47"/>
+      <c r="J15" s="121" t="s">
+        <v>475</v>
+      </c>
       <c r="K15" s="47"/>
       <c r="L15" s="47"/>
       <c r="M15" s="47"/>
@@ -5671,8 +5864,8 @@
       <c r="A16" s="62" t="s">
         <v>357</v>
       </c>
-      <c r="B16" s="104"/>
-      <c r="C16" s="104"/>
+      <c r="B16" s="109"/>
+      <c r="C16" s="109"/>
       <c r="D16" s="58">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -5687,7 +5880,9 @@
       <c r="I16" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J16" s="47"/>
+      <c r="J16" s="121" t="s">
+        <v>474</v>
+      </c>
       <c r="K16" s="47"/>
       <c r="L16" s="47"/>
       <c r="M16" s="47"/>
@@ -5710,8 +5905,8 @@
       <c r="A17" s="62" t="s">
         <v>358</v>
       </c>
-      <c r="B17" s="104"/>
-      <c r="C17" s="104"/>
+      <c r="B17" s="109"/>
+      <c r="C17" s="109"/>
       <c r="D17" s="58">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -5726,7 +5921,9 @@
       <c r="I17" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J17" s="47"/>
+      <c r="J17" s="121" t="s">
+        <v>473</v>
+      </c>
       <c r="K17" s="47"/>
       <c r="L17" s="47"/>
       <c r="M17" s="47"/>
@@ -5770,7 +5967,9 @@
       <c r="I18" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J18" s="47"/>
+      <c r="J18" s="121" t="s">
+        <v>472</v>
+      </c>
       <c r="K18" s="47"/>
       <c r="L18" s="47"/>
       <c r="M18" s="47"/>
@@ -5812,7 +6011,9 @@
       <c r="I19" s="71" t="s">
         <v>545</v>
       </c>
-      <c r="J19" s="47"/>
+      <c r="J19" s="121" t="s">
+        <v>1203</v>
+      </c>
       <c r="K19" s="47"/>
       <c r="L19" s="47"/>
       <c r="M19" s="47"/>
@@ -5835,11 +6036,11 @@
       <c r="A20" s="62" t="s">
         <v>370</v>
       </c>
-      <c r="B20" s="103">
+      <c r="B20" s="108">
         <f>B19+1</f>
         <v>43479</v>
       </c>
-      <c r="C20" s="103" t="str">
+      <c r="C20" s="108" t="str">
         <f t="shared" si="2"/>
         <v>Thứ 2</v>
       </c>
@@ -5857,7 +6058,9 @@
       <c r="I20" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J20" s="47"/>
+      <c r="J20" s="121" t="s">
+        <v>471</v>
+      </c>
       <c r="K20" s="47"/>
       <c r="L20" s="47"/>
       <c r="M20" s="47"/>
@@ -5880,8 +6083,8 @@
       <c r="A21" s="62" t="s">
         <v>359</v>
       </c>
-      <c r="B21" s="104"/>
-      <c r="C21" s="104"/>
+      <c r="B21" s="109"/>
+      <c r="C21" s="109"/>
       <c r="D21" s="58">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -5896,7 +6099,9 @@
       <c r="I21" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J21" s="47"/>
+      <c r="J21" s="117" t="s">
+        <v>369</v>
+      </c>
       <c r="K21" s="47"/>
       <c r="L21" s="47"/>
       <c r="M21" s="47"/>
@@ -5919,8 +6124,8 @@
       <c r="A22" s="62" t="s">
         <v>360</v>
       </c>
-      <c r="B22" s="104"/>
-      <c r="C22" s="104"/>
+      <c r="B22" s="109"/>
+      <c r="C22" s="109"/>
       <c r="D22" s="58">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -5935,7 +6140,9 @@
       <c r="I22" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J22" s="47"/>
+      <c r="J22" s="117" t="s">
+        <v>370</v>
+      </c>
       <c r="K22" s="47"/>
       <c r="L22" s="47"/>
       <c r="M22" s="47"/>
@@ -5980,7 +6187,9 @@
       <c r="I23" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J23" s="47"/>
+      <c r="J23" s="117" t="s">
+        <v>371</v>
+      </c>
       <c r="K23" s="47"/>
       <c r="L23" s="47"/>
       <c r="M23" s="47"/>
@@ -6023,7 +6232,9 @@
       <c r="I24" s="71" t="s">
         <v>545</v>
       </c>
-      <c r="J24" s="47"/>
+      <c r="J24" s="117" t="s">
+        <v>372</v>
+      </c>
       <c r="K24" s="47"/>
       <c r="L24" s="47"/>
       <c r="M24" s="47"/>
@@ -6042,7 +6253,7 @@
       <c r="Z24" s="47"/>
       <c r="AA24" s="47"/>
     </row>
-    <row r="25" spans="1:27" ht="15">
+    <row r="25" spans="1:27" ht="26.25">
       <c r="A25" s="62" t="s">
         <v>371</v>
       </c>
@@ -6068,7 +6279,9 @@
       <c r="I25" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J25" s="47"/>
+      <c r="J25" s="118" t="s">
+        <v>1204</v>
+      </c>
       <c r="K25" s="47"/>
       <c r="L25" s="47"/>
       <c r="M25" s="47"/>
@@ -6105,7 +6318,7 @@
       <c r="I26" s="71" t="s">
         <v>856</v>
       </c>
-      <c r="J26" s="47"/>
+      <c r="J26" s="117"/>
       <c r="K26" s="47"/>
       <c r="L26" s="47"/>
       <c r="M26" s="47"/>
@@ -6124,7 +6337,7 @@
       <c r="Z26" s="47"/>
       <c r="AA26" s="47"/>
     </row>
-    <row r="27" spans="1:27" ht="15.75" thickBot="1">
+    <row r="27" spans="1:27" ht="27" thickBot="1">
       <c r="A27" s="62" t="s">
         <v>362</v>
       </c>
@@ -6144,7 +6357,9 @@
       <c r="I27" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J27" s="47"/>
+      <c r="J27" s="118" t="s">
+        <v>1205</v>
+      </c>
       <c r="K27" s="47"/>
       <c r="L27" s="47"/>
       <c r="M27" s="47"/>
@@ -6188,7 +6403,9 @@
       <c r="I28" s="78" t="s">
         <v>545</v>
       </c>
-      <c r="J28" s="47"/>
+      <c r="J28" s="117" t="s">
+        <v>386</v>
+      </c>
       <c r="K28" s="47"/>
       <c r="L28" s="47"/>
       <c r="M28" s="47"/>
@@ -6226,7 +6443,9 @@
       <c r="G29" s="83"/>
       <c r="H29" s="83"/>
       <c r="I29" s="84"/>
-      <c r="J29" s="47"/>
+      <c r="J29" s="117" t="s">
+        <v>1206</v>
+      </c>
       <c r="K29" s="47"/>
       <c r="L29" s="47"/>
       <c r="M29" s="47"/>
@@ -6270,7 +6489,9 @@
       <c r="I30" s="84" t="s">
         <v>545</v>
       </c>
-      <c r="J30" s="47"/>
+      <c r="J30" s="122" t="s">
+        <v>463</v>
+      </c>
       <c r="K30" s="47"/>
       <c r="L30" s="47"/>
       <c r="M30" s="47"/>
@@ -6315,7 +6536,9 @@
       <c r="I31" s="84" t="s">
         <v>545</v>
       </c>
-      <c r="J31" s="47"/>
+      <c r="J31" s="119" t="s">
+        <v>1207</v>
+      </c>
       <c r="K31" s="47"/>
       <c r="L31" s="47"/>
       <c r="M31" s="47"/>
@@ -6419,21 +6642,21 @@
       <c r="AA33" s="47"/>
     </row>
     <row r="34" spans="1:27" ht="15">
-      <c r="A34" s="111" t="s">
+      <c r="A34" s="103" t="s">
         <v>400</v>
       </c>
-      <c r="B34" s="112">
+      <c r="B34" s="104">
         <f>B28 + 10</f>
         <v>43509</v>
       </c>
-      <c r="C34" s="112" t="str">
+      <c r="C34" s="104" t="str">
         <f>IF(WEEKDAY(B34,1)=1,"Chủ nhật","Thứ "&amp;WEEKDAY(B34,1))</f>
         <v>Thứ 4</v>
       </c>
-      <c r="D34" s="113">
+      <c r="D34" s="105">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E34" s="114"/>
+      <c r="E34" s="106"/>
       <c r="F34" s="83" t="s">
         <v>573</v>
       </c>
@@ -6675,21 +6898,21 @@
       <c r="AA39" s="47"/>
     </row>
     <row r="40" spans="1:27" ht="15">
-      <c r="A40" s="111" t="s">
+      <c r="A40" s="103" t="s">
         <v>401</v>
       </c>
-      <c r="B40" s="112">
+      <c r="B40" s="104">
         <f t="shared" si="6"/>
         <v>43511</v>
       </c>
-      <c r="C40" s="112" t="str">
+      <c r="C40" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 6</v>
       </c>
-      <c r="D40" s="113">
+      <c r="D40" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E40" s="114"/>
+      <c r="E40" s="106"/>
       <c r="F40" s="83" t="s">
         <v>573</v>
       </c>
@@ -6720,21 +6943,21 @@
       <c r="AA40" s="47"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" thickBot="1">
-      <c r="A41" s="111" t="s">
+      <c r="A41" s="103" t="s">
         <v>402</v>
       </c>
-      <c r="B41" s="112">
+      <c r="B41" s="104">
         <f t="shared" si="6"/>
         <v>43511</v>
       </c>
-      <c r="C41" s="112" t="str">
+      <c r="C41" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 6</v>
       </c>
-      <c r="D41" s="113">
+      <c r="D41" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E41" s="114"/>
+      <c r="E41" s="106"/>
       <c r="F41" s="83" t="s">
         <v>573</v>
       </c>
@@ -6849,21 +7072,21 @@
       <c r="AA43" s="47"/>
     </row>
     <row r="44" spans="1:27" ht="15.75" thickBot="1">
-      <c r="A44" s="111" t="s">
+      <c r="A44" s="103" t="s">
         <v>365</v>
       </c>
-      <c r="B44" s="112">
+      <c r="B44" s="104">
         <f>B37+ 2</f>
         <v>43512</v>
       </c>
-      <c r="C44" s="112" t="str">
+      <c r="C44" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 7</v>
       </c>
-      <c r="D44" s="113">
+      <c r="D44" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E44" s="114"/>
+      <c r="E44" s="106"/>
       <c r="F44" s="83" t="s">
         <v>573</v>
       </c>
@@ -6978,21 +7201,21 @@
       <c r="AA46" s="47"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" thickBot="1">
-      <c r="A47" s="111" t="s">
+      <c r="A47" s="103" t="s">
         <v>403</v>
       </c>
-      <c r="B47" s="115">
+      <c r="B47" s="107">
         <f>B45+1</f>
         <v>43513</v>
       </c>
-      <c r="C47" s="112" t="str">
+      <c r="C47" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Chủ nhật</v>
       </c>
-      <c r="D47" s="113">
+      <c r="D47" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E47" s="114"/>
+      <c r="E47" s="106"/>
       <c r="F47" s="83" t="s">
         <v>573</v>
       </c>
@@ -7058,21 +7281,21 @@
       <c r="AA48" s="47"/>
     </row>
     <row r="49" spans="1:27" ht="15">
-      <c r="A49" s="111" t="s">
+      <c r="A49" s="103" t="s">
         <v>404</v>
       </c>
-      <c r="B49" s="112">
+      <c r="B49" s="104">
         <f>B43 + 2</f>
         <v>43514</v>
       </c>
-      <c r="C49" s="112" t="str">
+      <c r="C49" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 2</v>
       </c>
-      <c r="D49" s="113">
+      <c r="D49" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E49" s="114"/>
+      <c r="E49" s="106"/>
       <c r="F49" s="83" t="s">
         <v>573</v>
       </c>
@@ -7181,21 +7404,21 @@
       <c r="AA51" s="47"/>
     </row>
     <row r="52" spans="1:27" ht="15">
-      <c r="A52" s="111" t="s">
+      <c r="A52" s="103" t="s">
         <v>367</v>
       </c>
-      <c r="B52" s="115">
+      <c r="B52" s="107">
         <f>B43+3</f>
         <v>43515</v>
       </c>
-      <c r="C52" s="112" t="str">
+      <c r="C52" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 3</v>
       </c>
-      <c r="D52" s="113">
+      <c r="D52" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E52" s="114"/>
+      <c r="E52" s="106"/>
       <c r="F52" s="83" t="s">
         <v>1065</v>
       </c>
@@ -7423,21 +7646,21 @@
       <c r="AA57" s="47"/>
     </row>
     <row r="58" spans="1:27" ht="15">
-      <c r="A58" s="111" t="s">
+      <c r="A58" s="103" t="s">
         <v>375</v>
       </c>
-      <c r="B58" s="112">
+      <c r="B58" s="104">
         <f t="shared" si="7"/>
         <v>43517</v>
       </c>
-      <c r="C58" s="112" t="str">
+      <c r="C58" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 5</v>
       </c>
-      <c r="D58" s="113">
+      <c r="D58" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E58" s="114"/>
+      <c r="E58" s="106"/>
       <c r="F58" s="83"/>
       <c r="G58" s="83"/>
       <c r="H58" s="83"/>
@@ -7462,21 +7685,21 @@
       <c r="AA58" s="47"/>
     </row>
     <row r="59" spans="1:27" ht="15.75" thickBot="1">
-      <c r="A59" s="111" t="s">
+      <c r="A59" s="103" t="s">
         <v>376</v>
       </c>
-      <c r="B59" s="112">
+      <c r="B59" s="104">
         <f t="shared" si="7"/>
         <v>43517</v>
       </c>
-      <c r="C59" s="112" t="str">
+      <c r="C59" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 5</v>
       </c>
-      <c r="D59" s="113">
+      <c r="D59" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E59" s="114"/>
+      <c r="E59" s="106"/>
       <c r="F59" s="83"/>
       <c r="G59" s="83"/>
       <c r="H59" s="83"/>
@@ -7540,21 +7763,21 @@
       <c r="AA60" s="47"/>
     </row>
     <row r="61" spans="1:27" ht="15">
-      <c r="A61" s="111" t="s">
+      <c r="A61" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="B61" s="112">
+      <c r="B61" s="104">
         <f>B59 + 1</f>
         <v>43518</v>
       </c>
-      <c r="C61" s="112" t="str">
+      <c r="C61" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 6</v>
       </c>
-      <c r="D61" s="113">
+      <c r="D61" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E61" s="114"/>
+      <c r="E61" s="106"/>
       <c r="F61" s="83"/>
       <c r="G61" s="83"/>
       <c r="H61" s="83"/>
@@ -7579,21 +7802,21 @@
       <c r="AA61" s="47"/>
     </row>
     <row r="62" spans="1:27" ht="15">
-      <c r="A62" s="111" t="s">
+      <c r="A62" s="103" t="s">
         <v>407</v>
       </c>
-      <c r="B62" s="112">
+      <c r="B62" s="104">
         <f>B59 + 1</f>
         <v>43518</v>
       </c>
-      <c r="C62" s="112" t="str">
+      <c r="C62" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 6</v>
       </c>
-      <c r="D62" s="113">
+      <c r="D62" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E62" s="114"/>
+      <c r="E62" s="106"/>
       <c r="F62" s="83"/>
       <c r="G62" s="83"/>
       <c r="H62" s="83"/>
@@ -7618,21 +7841,21 @@
       <c r="AA62" s="47"/>
     </row>
     <row r="63" spans="1:27" ht="15">
-      <c r="A63" s="111" t="s">
+      <c r="A63" s="103" t="s">
         <v>408</v>
       </c>
-      <c r="B63" s="112">
+      <c r="B63" s="104">
         <f>B59 +1</f>
         <v>43518</v>
       </c>
-      <c r="C63" s="112" t="str">
+      <c r="C63" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 6</v>
       </c>
-      <c r="D63" s="113">
+      <c r="D63" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E63" s="114"/>
+      <c r="E63" s="106"/>
       <c r="F63" s="83"/>
       <c r="G63" s="83"/>
       <c r="H63" s="83"/>
@@ -7698,21 +7921,21 @@
       <c r="AA64" s="47"/>
     </row>
     <row r="65" spans="1:27" ht="15">
-      <c r="A65" s="111" t="s">
+      <c r="A65" s="103" t="s">
         <v>379</v>
       </c>
-      <c r="B65" s="112">
+      <c r="B65" s="104">
         <f>B61 + 1</f>
         <v>43519</v>
       </c>
-      <c r="C65" s="112" t="str">
+      <c r="C65" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 7</v>
       </c>
-      <c r="D65" s="113">
+      <c r="D65" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E65" s="114"/>
+      <c r="E65" s="106"/>
       <c r="F65" s="83"/>
       <c r="G65" s="83"/>
       <c r="H65" s="83"/>
@@ -7737,21 +7960,21 @@
       <c r="AA65" s="47"/>
     </row>
     <row r="66" spans="1:27" ht="15">
-      <c r="A66" s="111" t="s">
+      <c r="A66" s="103" t="s">
         <v>380</v>
       </c>
-      <c r="B66" s="112">
+      <c r="B66" s="104">
         <f>B61 +1</f>
         <v>43519</v>
       </c>
-      <c r="C66" s="112" t="str">
+      <c r="C66" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 7</v>
       </c>
-      <c r="D66" s="113">
+      <c r="D66" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E66" s="114"/>
+      <c r="E66" s="106"/>
       <c r="F66" s="83"/>
       <c r="G66" s="83"/>
       <c r="H66" s="83"/>
@@ -7776,21 +7999,21 @@
       <c r="AA66" s="47"/>
     </row>
     <row r="67" spans="1:27" ht="15">
-      <c r="A67" s="111" t="s">
+      <c r="A67" s="103" t="s">
         <v>409</v>
       </c>
-      <c r="B67" s="112">
+      <c r="B67" s="104">
         <f t="shared" ref="B67:B73" si="8">B63 + 2</f>
         <v>43520</v>
       </c>
-      <c r="C67" s="112" t="str">
+      <c r="C67" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Chủ nhật</v>
       </c>
-      <c r="D67" s="113">
+      <c r="D67" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E67" s="114"/>
+      <c r="E67" s="106"/>
       <c r="F67" s="83"/>
       <c r="G67" s="83"/>
       <c r="H67" s="83"/>
@@ -7856,21 +8079,21 @@
       <c r="AA68" s="47"/>
     </row>
     <row r="69" spans="1:27" ht="15">
-      <c r="A69" s="111" t="s">
+      <c r="A69" s="103" t="s">
         <v>381</v>
       </c>
-      <c r="B69" s="112">
+      <c r="B69" s="104">
         <f>B65 + 1</f>
         <v>43520</v>
       </c>
-      <c r="C69" s="112" t="str">
+      <c r="C69" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Chủ nhật</v>
       </c>
-      <c r="D69" s="113">
+      <c r="D69" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E69" s="114"/>
+      <c r="E69" s="106"/>
       <c r="F69" s="83"/>
       <c r="G69" s="83"/>
       <c r="H69" s="83"/>
@@ -7895,21 +8118,21 @@
       <c r="AA69" s="47"/>
     </row>
     <row r="70" spans="1:27" ht="15">
-      <c r="A70" s="111" t="s">
+      <c r="A70" s="103" t="s">
         <v>382</v>
       </c>
-      <c r="B70" s="112">
+      <c r="B70" s="104">
         <f t="shared" si="8"/>
         <v>43521</v>
       </c>
-      <c r="C70" s="112" t="str">
+      <c r="C70" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 2</v>
       </c>
-      <c r="D70" s="113">
+      <c r="D70" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E70" s="114"/>
+      <c r="E70" s="106"/>
       <c r="F70" s="83"/>
       <c r="G70" s="83"/>
       <c r="H70" s="83"/>
@@ -7934,21 +8157,21 @@
       <c r="AA70" s="47"/>
     </row>
     <row r="71" spans="1:27" ht="15">
-      <c r="A71" s="111" t="s">
+      <c r="A71" s="103" t="s">
         <v>383</v>
       </c>
-      <c r="B71" s="112">
+      <c r="B71" s="104">
         <f>B67 + 1</f>
         <v>43521</v>
       </c>
-      <c r="C71" s="112" t="str">
+      <c r="C71" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 2</v>
       </c>
-      <c r="D71" s="113">
+      <c r="D71" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E71" s="114"/>
+      <c r="E71" s="106"/>
       <c r="F71" s="83"/>
       <c r="G71" s="83"/>
       <c r="H71" s="83"/>
@@ -7973,21 +8196,21 @@
       <c r="AA71" s="47"/>
     </row>
     <row r="72" spans="1:27" ht="15">
-      <c r="A72" s="111" t="s">
+      <c r="A72" s="103" t="s">
         <v>410</v>
       </c>
-      <c r="B72" s="112">
+      <c r="B72" s="104">
         <f>B68 + 1</f>
         <v>43521</v>
       </c>
-      <c r="C72" s="112" t="str">
+      <c r="C72" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 2</v>
       </c>
-      <c r="D72" s="113">
+      <c r="D72" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E72" s="114"/>
+      <c r="E72" s="106"/>
       <c r="F72" s="83"/>
       <c r="G72" s="83"/>
       <c r="H72" s="83"/>
@@ -8012,21 +8235,21 @@
       <c r="AA72" s="47"/>
     </row>
     <row r="73" spans="1:27" ht="15">
-      <c r="A73" s="111" t="s">
+      <c r="A73" s="103" t="s">
         <v>411</v>
       </c>
-      <c r="B73" s="112">
+      <c r="B73" s="104">
         <f t="shared" si="8"/>
         <v>43522</v>
       </c>
-      <c r="C73" s="112" t="str">
+      <c r="C73" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 3</v>
       </c>
-      <c r="D73" s="113">
+      <c r="D73" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E73" s="114"/>
+      <c r="E73" s="106"/>
       <c r="F73" s="83"/>
       <c r="G73" s="83"/>
       <c r="H73" s="83"/>
@@ -8051,21 +8274,21 @@
       <c r="AA73" s="47"/>
     </row>
     <row r="74" spans="1:27" ht="15">
-      <c r="A74" s="111" t="s">
+      <c r="A74" s="103" t="s">
         <v>384</v>
       </c>
-      <c r="B74" s="112">
+      <c r="B74" s="104">
         <f>B70 + 1</f>
         <v>43522</v>
       </c>
-      <c r="C74" s="112" t="str">
+      <c r="C74" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 3</v>
       </c>
-      <c r="D74" s="113">
+      <c r="D74" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E74" s="114"/>
+      <c r="E74" s="106"/>
       <c r="F74" s="83"/>
       <c r="G74" s="83"/>
       <c r="H74" s="83"/>
@@ -8090,21 +8313,21 @@
       <c r="AA74" s="47"/>
     </row>
     <row r="75" spans="1:27" ht="15">
-      <c r="A75" s="111" t="s">
+      <c r="A75" s="103" t="s">
         <v>385</v>
       </c>
-      <c r="B75" s="112">
+      <c r="B75" s="104">
         <f>B71 + 1</f>
         <v>43522</v>
       </c>
-      <c r="C75" s="112" t="str">
+      <c r="C75" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 3</v>
       </c>
-      <c r="D75" s="113">
+      <c r="D75" s="105">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E75" s="114"/>
+      <c r="E75" s="106"/>
       <c r="F75" s="83"/>
       <c r="G75" s="83"/>
       <c r="H75" s="83"/>
@@ -8129,7 +8352,7 @@
       <c r="AA75" s="47"/>
     </row>
     <row r="76" spans="1:27" ht="15">
-      <c r="A76" s="79" t="s">
+      <c r="A76" s="98" t="s">
         <v>386</v>
       </c>
       <c r="B76" s="80">
@@ -8170,7 +8393,7 @@
       <c r="AA76" s="47"/>
     </row>
     <row r="77" spans="1:27" ht="15">
-      <c r="A77" s="79" t="s">
+      <c r="A77" s="98" t="s">
         <v>387</v>
       </c>
       <c r="B77" s="80">
@@ -8211,21 +8434,21 @@
       <c r="AA77" s="47"/>
     </row>
     <row r="78" spans="1:27" ht="15">
-      <c r="A78" s="111" t="s">
+      <c r="A78" s="103" t="s">
         <v>388</v>
       </c>
-      <c r="B78" s="112">
+      <c r="B78" s="104">
         <f>B73 + 3</f>
         <v>43525</v>
       </c>
-      <c r="C78" s="112" t="str">
+      <c r="C78" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 6</v>
       </c>
-      <c r="D78" s="113">
+      <c r="D78" s="105">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E78" s="114"/>
+      <c r="E78" s="106"/>
       <c r="F78" s="83"/>
       <c r="G78" s="83"/>
       <c r="H78" s="83"/>
@@ -8250,21 +8473,21 @@
       <c r="AA78" s="47"/>
     </row>
     <row r="79" spans="1:27" ht="15">
-      <c r="A79" s="111" t="s">
+      <c r="A79" s="103" t="s">
         <v>389</v>
       </c>
-      <c r="B79" s="112">
+      <c r="B79" s="104">
         <f>B75 + 4</f>
         <v>43526</v>
       </c>
-      <c r="C79" s="112" t="str">
+      <c r="C79" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 7</v>
       </c>
-      <c r="D79" s="113">
+      <c r="D79" s="105">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E79" s="114"/>
+      <c r="E79" s="106"/>
       <c r="F79" s="83"/>
       <c r="G79" s="83"/>
       <c r="H79" s="83"/>
@@ -31816,11 +32039,14 @@
     <hyperlink ref="A50" location="'Mock Exam 6'!A1" display="Mock Exam 6" xr:uid="{21129F36-5031-4CB2-B056-ED699CEDB28A}"/>
     <hyperlink ref="H46" location="'Initiating 1'!A1" display="Initiating 1" xr:uid="{867C4E7E-1E58-4BC8-BBC0-805FB2FC6C0D}"/>
     <hyperlink ref="H32" location="'Monitoring 11'!A1" display="Monitoring 11" xr:uid="{4C83CE24-4F77-408F-8C88-192BFFAE7BA9}"/>
+    <hyperlink ref="A77" location="'Full test 1'!A1" display="Full Test 1" xr:uid="{4523928A-4B63-4171-8AC8-43FCA3957AD0}"/>
+    <hyperlink ref="A76" location="'Mock Exam 18'!A1" display="Mock Exam 18" xr:uid="{AAAD6C9F-C7E5-4721-A8F7-BCDBDC617092}"/>
+    <hyperlink ref="J31" location="Procurement!A1" display="Procurement" xr:uid="{B582D725-D656-4BC8-BC38-EE165D67735C}"/>
+    <hyperlink ref="J30" location="Resource!A1" display="Resource" xr:uid="{1558CF88-E21B-447A-9F90-5E20C72FCB65}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -32134,8 +32360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE7AA35E-BA94-465D-947F-048E2F692024}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32189,7 +32415,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="45">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -32198,11 +32424,11 @@
         <v>4</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="60">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -32211,7 +32437,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>550</v>
       </c>
     </row>
@@ -36214,8 +36440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB276F1D-E283-4EC7-864D-9C4AF9A2426A}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -41555,8 +41781,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -50032,152 +50258,152 @@
       <c r="A1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="105" t="s">
+      <c r="B1" s="110" t="s">
         <v>212</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="107"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="112"/>
     </row>
     <row r="2" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="110" t="s">
         <v>213</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106"/>
-      <c r="J2" s="106"/>
-      <c r="K2" s="107"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="112"/>
     </row>
     <row r="3" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A3" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="110" t="s">
         <v>214</v>
       </c>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="106"/>
-      <c r="H3" s="106"/>
-      <c r="I3" s="106"/>
-      <c r="J3" s="106"/>
-      <c r="K3" s="107"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="112"/>
     </row>
     <row r="4" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A4" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="105" t="s">
+      <c r="B4" s="110" t="s">
         <v>215</v>
       </c>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
-      <c r="J4" s="106"/>
-      <c r="K4" s="107"/>
+      <c r="C4" s="111"/>
+      <c r="D4" s="111"/>
+      <c r="E4" s="111"/>
+      <c r="F4" s="111"/>
+      <c r="G4" s="111"/>
+      <c r="H4" s="111"/>
+      <c r="I4" s="111"/>
+      <c r="J4" s="111"/>
+      <c r="K4" s="112"/>
     </row>
     <row r="5" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A5" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="110" t="s">
         <v>216</v>
       </c>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="107"/>
+      <c r="C5" s="111"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="111"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="112"/>
     </row>
     <row r="6" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="105" t="s">
+      <c r="B6" s="110" t="s">
         <v>217</v>
       </c>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
-      <c r="J6" s="106"/>
-      <c r="K6" s="107"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="111"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="111"/>
+      <c r="K6" s="112"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="105" t="s">
+      <c r="B7" s="110" t="s">
         <v>218</v>
       </c>
-      <c r="C7" s="106"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106"/>
-      <c r="G7" s="106"/>
-      <c r="H7" s="106"/>
-      <c r="I7" s="106"/>
-      <c r="J7" s="106"/>
-      <c r="K7" s="107"/>
+      <c r="C7" s="111"/>
+      <c r="D7" s="111"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="111"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
+      <c r="J7" s="111"/>
+      <c r="K7" s="112"/>
     </row>
     <row r="8" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A8" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="B8" s="105" t="s">
+      <c r="B8" s="110" t="s">
         <v>219</v>
       </c>
-      <c r="C8" s="106"/>
-      <c r="D8" s="106"/>
-      <c r="E8" s="106"/>
-      <c r="F8" s="106"/>
-      <c r="G8" s="106"/>
-      <c r="H8" s="106"/>
-      <c r="I8" s="106"/>
-      <c r="J8" s="106"/>
-      <c r="K8" s="107"/>
+      <c r="C8" s="111"/>
+      <c r="D8" s="111"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="111"/>
+      <c r="J8" s="111"/>
+      <c r="K8" s="112"/>
     </row>
     <row r="9" spans="1:11" ht="99.75" customHeight="1" thickBot="1">
       <c r="A9" s="10"/>
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="113" t="s">
         <v>220</v>
       </c>
-      <c r="C9" s="109"/>
-      <c r="D9" s="109"/>
-      <c r="E9" s="109"/>
-      <c r="F9" s="109"/>
-      <c r="G9" s="109"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="109"/>
-      <c r="J9" s="109"/>
-      <c r="K9" s="110"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="114"/>
+      <c r="H9" s="114"/>
+      <c r="I9" s="114"/>
+      <c r="J9" s="114"/>
+      <c r="K9" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -50210,222 +50436,222 @@
       <c r="A1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="105" t="s">
+      <c r="B1" s="110" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="107"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="112"/>
     </row>
     <row r="2" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="110" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106"/>
-      <c r="J2" s="106"/>
-      <c r="K2" s="107"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="112"/>
     </row>
     <row r="3" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A3" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="106"/>
-      <c r="H3" s="106"/>
-      <c r="I3" s="106"/>
-      <c r="J3" s="106"/>
-      <c r="K3" s="107"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="112"/>
     </row>
     <row r="4" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A4" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="105" t="s">
+      <c r="B4" s="110" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
-      <c r="J4" s="106"/>
-      <c r="K4" s="107"/>
+      <c r="C4" s="111"/>
+      <c r="D4" s="111"/>
+      <c r="E4" s="111"/>
+      <c r="F4" s="111"/>
+      <c r="G4" s="111"/>
+      <c r="H4" s="111"/>
+      <c r="I4" s="111"/>
+      <c r="J4" s="111"/>
+      <c r="K4" s="112"/>
     </row>
     <row r="5" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A5" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="110" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="107"/>
+      <c r="C5" s="111"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="111"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="112"/>
     </row>
     <row r="6" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="105" t="s">
+      <c r="B6" s="110" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
-      <c r="J6" s="106"/>
-      <c r="K6" s="107"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="111"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="111"/>
+      <c r="K6" s="112"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="105" t="s">
+      <c r="B7" s="110" t="s">
         <v>136</v>
       </c>
-      <c r="C7" s="106"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106"/>
-      <c r="G7" s="106"/>
-      <c r="H7" s="106"/>
-      <c r="I7" s="106"/>
-      <c r="J7" s="106"/>
-      <c r="K7" s="107"/>
+      <c r="C7" s="111"/>
+      <c r="D7" s="111"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="111"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
+      <c r="J7" s="111"/>
+      <c r="K7" s="112"/>
     </row>
     <row r="8" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A8" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="B8" s="105" t="s">
+      <c r="B8" s="110" t="s">
         <v>138</v>
       </c>
-      <c r="C8" s="106"/>
-      <c r="D8" s="106"/>
-      <c r="E8" s="106"/>
-      <c r="F8" s="106"/>
-      <c r="G8" s="106"/>
-      <c r="H8" s="106"/>
-      <c r="I8" s="106"/>
-      <c r="J8" s="106"/>
-      <c r="K8" s="107"/>
+      <c r="C8" s="111"/>
+      <c r="D8" s="111"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="111"/>
+      <c r="J8" s="111"/>
+      <c r="K8" s="112"/>
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1" thickBot="1">
       <c r="A9" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="B9" s="105" t="s">
+      <c r="B9" s="110" t="s">
         <v>140</v>
       </c>
-      <c r="C9" s="106"/>
-      <c r="D9" s="106"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="106"/>
-      <c r="G9" s="106"/>
-      <c r="H9" s="106"/>
-      <c r="I9" s="106"/>
-      <c r="J9" s="106"/>
-      <c r="K9" s="107"/>
+      <c r="C9" s="111"/>
+      <c r="D9" s="111"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="111"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="111"/>
+      <c r="J9" s="111"/>
+      <c r="K9" s="112"/>
     </row>
     <row r="10" spans="1:11" ht="60" customHeight="1" thickBot="1">
       <c r="A10" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="B10" s="105" t="s">
+      <c r="B10" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="C10" s="106"/>
-      <c r="D10" s="106"/>
-      <c r="E10" s="106"/>
-      <c r="F10" s="106"/>
-      <c r="G10" s="106"/>
-      <c r="H10" s="106"/>
-      <c r="I10" s="106"/>
-      <c r="J10" s="106"/>
-      <c r="K10" s="107"/>
+      <c r="C10" s="111"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="111"/>
+      <c r="F10" s="111"/>
+      <c r="G10" s="111"/>
+      <c r="H10" s="111"/>
+      <c r="I10" s="111"/>
+      <c r="J10" s="111"/>
+      <c r="K10" s="112"/>
     </row>
     <row r="11" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A11" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="B11" s="105" t="s">
+      <c r="B11" s="110" t="s">
         <v>144</v>
       </c>
-      <c r="C11" s="106"/>
-      <c r="D11" s="106"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="106"/>
-      <c r="G11" s="106"/>
-      <c r="H11" s="106"/>
-      <c r="I11" s="106"/>
-      <c r="J11" s="106"/>
-      <c r="K11" s="107"/>
+      <c r="C11" s="111"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="111"/>
+      <c r="G11" s="111"/>
+      <c r="H11" s="111"/>
+      <c r="I11" s="111"/>
+      <c r="J11" s="111"/>
+      <c r="K11" s="112"/>
     </row>
     <row r="12" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A12" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="B12" s="105" t="s">
+      <c r="B12" s="110" t="s">
         <v>146</v>
       </c>
-      <c r="C12" s="106"/>
-      <c r="D12" s="106"/>
-      <c r="E12" s="106"/>
-      <c r="F12" s="106"/>
-      <c r="G12" s="106"/>
-      <c r="H12" s="106"/>
-      <c r="I12" s="106"/>
-      <c r="J12" s="106"/>
-      <c r="K12" s="107"/>
+      <c r="C12" s="111"/>
+      <c r="D12" s="111"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="111"/>
+      <c r="G12" s="111"/>
+      <c r="H12" s="111"/>
+      <c r="I12" s="111"/>
+      <c r="J12" s="111"/>
+      <c r="K12" s="112"/>
     </row>
     <row r="13" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A13" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B13" s="105" t="s">
+      <c r="B13" s="110" t="s">
         <v>148</v>
       </c>
-      <c r="C13" s="106"/>
-      <c r="D13" s="106"/>
-      <c r="E13" s="106"/>
-      <c r="F13" s="106"/>
-      <c r="G13" s="106"/>
-      <c r="H13" s="106"/>
-      <c r="I13" s="106"/>
-      <c r="J13" s="106"/>
-      <c r="K13" s="107"/>
+      <c r="C13" s="111"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="111"/>
+      <c r="K13" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -50462,120 +50688,120 @@
       <c r="A1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="105" t="s">
+      <c r="B1" s="110" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="107"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="112"/>
     </row>
     <row r="2" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="110" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106"/>
-      <c r="J2" s="106"/>
-      <c r="K2" s="107"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="112"/>
     </row>
     <row r="3" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A3" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="110" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="106"/>
-      <c r="H3" s="106"/>
-      <c r="I3" s="106"/>
-      <c r="J3" s="106"/>
-      <c r="K3" s="107"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="112"/>
     </row>
     <row r="4" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A4" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="105" t="s">
+      <c r="B4" s="110" t="s">
         <v>155</v>
       </c>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
-      <c r="J4" s="106"/>
-      <c r="K4" s="107"/>
+      <c r="C4" s="111"/>
+      <c r="D4" s="111"/>
+      <c r="E4" s="111"/>
+      <c r="F4" s="111"/>
+      <c r="G4" s="111"/>
+      <c r="H4" s="111"/>
+      <c r="I4" s="111"/>
+      <c r="J4" s="111"/>
+      <c r="K4" s="112"/>
     </row>
     <row r="5" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A5" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="110" t="s">
         <v>152</v>
       </c>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="107"/>
+      <c r="C5" s="111"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="111"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="112"/>
     </row>
     <row r="6" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="105" t="s">
+      <c r="B6" s="110" t="s">
         <v>153</v>
       </c>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
-      <c r="J6" s="106"/>
-      <c r="K6" s="107"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="111"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="111"/>
+      <c r="K6" s="112"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="105" t="s">
+      <c r="B7" s="110" t="s">
         <v>154</v>
       </c>
-      <c r="C7" s="106"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106"/>
-      <c r="G7" s="106"/>
-      <c r="H7" s="106"/>
-      <c r="I7" s="106"/>
-      <c r="J7" s="106"/>
-      <c r="K7" s="107"/>
+      <c r="C7" s="111"/>
+      <c r="D7" s="111"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="111"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
+      <c r="J7" s="111"/>
+      <c r="K7" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -50607,120 +50833,120 @@
       <c r="A1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="105" t="s">
+      <c r="B1" s="110" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="107"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="112"/>
     </row>
     <row r="2" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="110" t="s">
         <v>157</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106"/>
-      <c r="J2" s="106"/>
-      <c r="K2" s="107"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="112"/>
     </row>
     <row r="3" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A3" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="110" t="s">
         <v>158</v>
       </c>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="106"/>
-      <c r="H3" s="106"/>
-      <c r="I3" s="106"/>
-      <c r="J3" s="106"/>
-      <c r="K3" s="107"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="112"/>
     </row>
     <row r="4" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A4" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="105" t="s">
+      <c r="B4" s="110" t="s">
         <v>159</v>
       </c>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
-      <c r="J4" s="106"/>
-      <c r="K4" s="107"/>
+      <c r="C4" s="111"/>
+      <c r="D4" s="111"/>
+      <c r="E4" s="111"/>
+      <c r="F4" s="111"/>
+      <c r="G4" s="111"/>
+      <c r="H4" s="111"/>
+      <c r="I4" s="111"/>
+      <c r="J4" s="111"/>
+      <c r="K4" s="112"/>
     </row>
     <row r="5" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A5" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="110" t="s">
         <v>160</v>
       </c>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="107"/>
+      <c r="C5" s="111"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="111"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="112"/>
     </row>
     <row r="6" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="105" t="s">
+      <c r="B6" s="110" t="s">
         <v>161</v>
       </c>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
-      <c r="J6" s="106"/>
-      <c r="K6" s="107"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="111"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="111"/>
+      <c r="K6" s="112"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="105" t="s">
+      <c r="B7" s="110" t="s">
         <v>162</v>
       </c>
-      <c r="C7" s="106"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106"/>
-      <c r="G7" s="106"/>
-      <c r="H7" s="106"/>
-      <c r="I7" s="106"/>
-      <c r="J7" s="106"/>
-      <c r="K7" s="107"/>
+      <c r="C7" s="111"/>
+      <c r="D7" s="111"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="111"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
+      <c r="J7" s="111"/>
+      <c r="K7" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -51417,135 +51643,135 @@
       <c r="A1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="105" t="s">
+      <c r="B1" s="110" t="s">
         <v>221</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="107"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="112"/>
     </row>
     <row r="2" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="110" t="s">
         <v>222</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106"/>
-      <c r="J2" s="106"/>
-      <c r="K2" s="107"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="112"/>
     </row>
     <row r="3" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A3" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="110" t="s">
         <v>223</v>
       </c>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="106"/>
-      <c r="H3" s="106"/>
-      <c r="I3" s="106"/>
-      <c r="J3" s="106"/>
-      <c r="K3" s="107"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="112"/>
     </row>
     <row r="4" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A4" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="105" t="s">
+      <c r="B4" s="110" t="s">
         <v>224</v>
       </c>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
-      <c r="J4" s="106"/>
-      <c r="K4" s="107"/>
+      <c r="C4" s="111"/>
+      <c r="D4" s="111"/>
+      <c r="E4" s="111"/>
+      <c r="F4" s="111"/>
+      <c r="G4" s="111"/>
+      <c r="H4" s="111"/>
+      <c r="I4" s="111"/>
+      <c r="J4" s="111"/>
+      <c r="K4" s="112"/>
     </row>
     <row r="5" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A5" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="110" t="s">
         <v>225</v>
       </c>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="107"/>
+      <c r="C5" s="111"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="111"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="112"/>
     </row>
     <row r="6" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="105" t="s">
+      <c r="B6" s="110" t="s">
         <v>226</v>
       </c>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
-      <c r="J6" s="106"/>
-      <c r="K6" s="107"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="111"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="111"/>
+      <c r="K6" s="112"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="105" t="s">
+      <c r="B7" s="110" t="s">
         <v>227</v>
       </c>
-      <c r="C7" s="106"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106"/>
-      <c r="G7" s="106"/>
-      <c r="H7" s="106"/>
-      <c r="I7" s="106"/>
-      <c r="J7" s="106"/>
-      <c r="K7" s="107"/>
+      <c r="C7" s="111"/>
+      <c r="D7" s="111"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="111"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
+      <c r="J7" s="111"/>
+      <c r="K7" s="112"/>
     </row>
     <row r="8" spans="1:11" ht="150.75" customHeight="1" thickBot="1">
       <c r="A8" s="10"/>
-      <c r="B8" s="108" t="s">
+      <c r="B8" s="113" t="s">
         <v>228</v>
       </c>
-      <c r="C8" s="109"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="109"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="109"/>
-      <c r="K8" s="110"/>
+      <c r="C8" s="114"/>
+      <c r="D8" s="114"/>
+      <c r="E8" s="114"/>
+      <c r="F8" s="114"/>
+      <c r="G8" s="114"/>
+      <c r="H8" s="114"/>
+      <c r="I8" s="114"/>
+      <c r="J8" s="114"/>
+      <c r="K8" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -51893,6 +52119,1677 @@
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F383373-F0A3-479D-A7AB-FEC4B3E1DC8F}">
+  <dimension ref="A1:G201"/>
+  <sheetViews>
+    <sheetView topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="D201" sqref="D201"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" customWidth="1"/>
+    <col min="6" max="6" width="79" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="25.5">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="15"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="15"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:7" ht="30">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="15" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="75">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="15" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G7" s="57"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="15"/>
+      <c r="G10" s="57"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="15" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="1:7" ht="30">
+      <c r="A16" s="8">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E16" s="15"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="8">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="1:5" ht="45">
+      <c r="A20" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="8">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="8">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="8">
+        <v>22</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:5" ht="45">
+      <c r="A24" s="8">
+        <v>23</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="8">
+        <v>24</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="8">
+        <v>25</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="8">
+        <v>26</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:5" ht="60">
+      <c r="A28" s="8">
+        <v>27</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="8">
+        <v>28</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="8">
+        <v>29</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="15"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="8">
+        <v>30</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="15"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="8">
+        <v>31</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="15"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="8">
+        <v>32</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="15"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="8">
+        <v>33</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="15"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="8">
+        <v>34</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="15"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="8">
+        <v>35</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="15"/>
+    </row>
+    <row r="37" spans="1:5" ht="60">
+      <c r="A37" s="8">
+        <v>36</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E37" s="15"/>
+    </row>
+    <row r="38" spans="1:5" ht="75">
+      <c r="A38" s="8">
+        <v>37</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="8">
+        <v>38</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="15"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="8">
+        <v>39</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="15"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="8">
+        <v>40</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="15"/>
+    </row>
+    <row r="42" spans="1:5" ht="30">
+      <c r="A42" s="8">
+        <v>41</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E42" s="15"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="8">
+        <v>42</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="15"/>
+    </row>
+    <row r="44" spans="1:5" ht="30">
+      <c r="A44" s="8">
+        <v>43</v>
+      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E44" s="15"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="8">
+        <v>44</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="15"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="8">
+        <v>45</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="15"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="8">
+        <v>46</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="15"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="8">
+        <v>47</v>
+      </c>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="15"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="8">
+        <v>48</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="15"/>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="8">
+        <v>49</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="15"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="8">
+        <v>50</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="15"/>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="8">
+        <v>51</v>
+      </c>
+      <c r="C52" s="8"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="8">
+        <v>52</v>
+      </c>
+      <c r="C53" s="8"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="8">
+        <v>53</v>
+      </c>
+      <c r="C54" s="8"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="8">
+        <v>54</v>
+      </c>
+      <c r="C55" s="8"/>
+    </row>
+    <row r="56" spans="1:5" ht="45">
+      <c r="A56" s="8">
+        <v>55</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="65" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="8">
+        <v>56</v>
+      </c>
+      <c r="C57" s="8"/>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="8">
+        <v>57</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="8">
+        <v>58</v>
+      </c>
+      <c r="C59" s="8"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="8">
+        <v>59</v>
+      </c>
+      <c r="C60" s="8"/>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="8">
+        <v>60</v>
+      </c>
+      <c r="C61" s="8"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="8">
+        <v>61</v>
+      </c>
+      <c r="C62" s="8"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="8">
+        <v>62</v>
+      </c>
+      <c r="C63" s="8"/>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="8">
+        <v>63</v>
+      </c>
+      <c r="C64" s="8"/>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="8">
+        <v>64</v>
+      </c>
+      <c r="C65" s="8"/>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="8">
+        <v>65</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="8">
+        <v>66</v>
+      </c>
+      <c r="C67" s="8"/>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="8">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="8">
+        <v>68</v>
+      </c>
+      <c r="D69" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="8">
+        <v>69</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="8">
+        <v>71</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="8">
+        <v>72</v>
+      </c>
+      <c r="C73" s="8"/>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="8">
+        <v>73</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="8">
+        <v>74</v>
+      </c>
+      <c r="C75" s="8"/>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="8">
+        <v>75</v>
+      </c>
+      <c r="C76" s="8"/>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="8">
+        <v>76</v>
+      </c>
+      <c r="C77" s="8"/>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="8">
+        <v>77</v>
+      </c>
+      <c r="C78" s="8"/>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="8">
+        <v>78</v>
+      </c>
+      <c r="C79" s="8"/>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="8">
+        <v>79</v>
+      </c>
+      <c r="C80" s="8"/>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="8">
+        <v>80</v>
+      </c>
+      <c r="C81" s="8"/>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="8">
+        <v>81</v>
+      </c>
+      <c r="C82" s="8"/>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="8">
+        <v>82</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="8">
+        <v>83</v>
+      </c>
+      <c r="C84" s="8"/>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="8">
+        <v>84</v>
+      </c>
+      <c r="C85" s="8"/>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="8">
+        <v>85</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="8">
+        <v>86</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D87" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="8">
+        <v>87</v>
+      </c>
+      <c r="C88" s="8"/>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="8">
+        <v>88</v>
+      </c>
+      <c r="C89" s="8"/>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="8">
+        <v>89</v>
+      </c>
+      <c r="C90" s="8"/>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="8">
+        <v>90</v>
+      </c>
+      <c r="C91" s="8"/>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="8">
+        <v>91</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D92" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="8">
+        <v>92</v>
+      </c>
+      <c r="C93" s="8"/>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="8">
+        <v>93</v>
+      </c>
+      <c r="C94" s="8"/>
+    </row>
+    <row r="95" spans="1:4" ht="90">
+      <c r="A95" s="8">
+        <v>94</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D95" s="65" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="8">
+        <v>95</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D96" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="8">
+        <v>96</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="8">
+        <v>97</v>
+      </c>
+      <c r="C98" s="8"/>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="8">
+        <v>98</v>
+      </c>
+      <c r="C99" s="8"/>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="8">
+        <v>99</v>
+      </c>
+      <c r="C100" s="8"/>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="8">
+        <v>100</v>
+      </c>
+      <c r="C101" s="8"/>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="8">
+        <v>101</v>
+      </c>
+      <c r="C102" s="8"/>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="8">
+        <v>102</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D103" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="8">
+        <v>103</v>
+      </c>
+      <c r="C104" s="8"/>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="8">
+        <v>104</v>
+      </c>
+      <c r="C105" s="8"/>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="8">
+        <v>105</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D106" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="8">
+        <v>106</v>
+      </c>
+      <c r="C107" s="8"/>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="8">
+        <v>107</v>
+      </c>
+      <c r="C108" s="8"/>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="8">
+        <v>108</v>
+      </c>
+      <c r="C109" s="8"/>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="8">
+        <v>109</v>
+      </c>
+      <c r="C110" s="8"/>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="8">
+        <v>110</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D111" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="8">
+        <v>111</v>
+      </c>
+      <c r="C112" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D112" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" s="8">
+        <v>112</v>
+      </c>
+      <c r="C113" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D113" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" s="8">
+        <v>113</v>
+      </c>
+      <c r="C114" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D114" s="45" t="s">
+        <v>1172</v>
+      </c>
+      <c r="E114" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="8">
+        <v>114</v>
+      </c>
+      <c r="C115" s="8"/>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" s="8">
+        <v>115</v>
+      </c>
+      <c r="C116" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D116" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" s="8">
+        <v>116</v>
+      </c>
+      <c r="C117" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D117" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" s="8">
+        <v>117</v>
+      </c>
+      <c r="C118" s="8"/>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" s="8">
+        <v>118</v>
+      </c>
+      <c r="C119" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D119" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" s="8">
+        <v>119</v>
+      </c>
+      <c r="C120" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D120" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" s="8">
+        <v>120</v>
+      </c>
+      <c r="C121" s="8"/>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" s="8">
+        <v>121</v>
+      </c>
+      <c r="C122" s="8"/>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" s="8">
+        <v>122</v>
+      </c>
+      <c r="C123" s="8"/>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" s="8">
+        <v>123</v>
+      </c>
+      <c r="C124" s="8"/>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" s="8">
+        <v>124</v>
+      </c>
+      <c r="C125" s="8"/>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" s="8">
+        <v>125</v>
+      </c>
+      <c r="C126" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D126" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" s="8">
+        <v>126</v>
+      </c>
+      <c r="C127" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D127" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" s="8">
+        <v>127</v>
+      </c>
+      <c r="C128" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D128" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" s="8">
+        <v>128</v>
+      </c>
+      <c r="C129" s="8"/>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" s="8">
+        <v>129</v>
+      </c>
+      <c r="C130" s="8"/>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" s="8">
+        <v>130</v>
+      </c>
+      <c r="C131" s="8"/>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" s="8">
+        <v>131</v>
+      </c>
+      <c r="C132" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" s="8">
+        <v>132</v>
+      </c>
+      <c r="C133" s="8"/>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" s="8">
+        <v>133</v>
+      </c>
+      <c r="C134" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D134" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E134" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" s="8">
+        <v>134</v>
+      </c>
+      <c r="C135" s="8"/>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" s="8">
+        <v>135</v>
+      </c>
+      <c r="C136" s="8"/>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" s="8">
+        <v>136</v>
+      </c>
+      <c r="C137" s="8"/>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" s="8">
+        <v>137</v>
+      </c>
+      <c r="C138" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D138" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" s="8">
+        <v>138</v>
+      </c>
+      <c r="C139" s="8"/>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" s="8">
+        <v>139</v>
+      </c>
+      <c r="C140" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D140" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" s="8">
+        <v>140</v>
+      </c>
+      <c r="C141" s="8"/>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" s="8">
+        <v>141</v>
+      </c>
+      <c r="C142" s="8"/>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" s="8">
+        <v>142</v>
+      </c>
+      <c r="C143" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D143" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" s="8">
+        <v>143</v>
+      </c>
+      <c r="C144" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D144" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="8">
+        <v>144</v>
+      </c>
+      <c r="C145" s="8"/>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="8">
+        <v>145</v>
+      </c>
+      <c r="C146" s="8"/>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="8">
+        <v>146</v>
+      </c>
+      <c r="C147" s="8"/>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="8">
+        <v>147</v>
+      </c>
+      <c r="C148" s="8"/>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="8">
+        <v>148</v>
+      </c>
+      <c r="C149" s="8"/>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="8">
+        <v>149</v>
+      </c>
+      <c r="C150" s="8"/>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="8">
+        <v>150</v>
+      </c>
+      <c r="C151" s="8"/>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="8">
+        <v>151</v>
+      </c>
+      <c r="C152" s="8"/>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" s="8">
+        <v>152</v>
+      </c>
+      <c r="C153" s="8"/>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" s="8">
+        <v>153</v>
+      </c>
+      <c r="C154" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D154" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" s="8">
+        <v>154</v>
+      </c>
+      <c r="C155" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D155" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" s="8">
+        <v>155</v>
+      </c>
+      <c r="C156" s="8"/>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="8">
+        <v>156</v>
+      </c>
+      <c r="C157" s="8"/>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" s="8">
+        <v>157</v>
+      </c>
+      <c r="C158" s="8"/>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" s="8">
+        <v>158</v>
+      </c>
+      <c r="C159" s="8"/>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" s="8">
+        <v>159</v>
+      </c>
+      <c r="C160" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D160" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" s="8">
+        <v>160</v>
+      </c>
+      <c r="C161" s="8"/>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" s="8">
+        <v>161</v>
+      </c>
+      <c r="C162" s="8"/>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" s="8">
+        <v>162</v>
+      </c>
+      <c r="C163" s="8"/>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" s="8">
+        <v>163</v>
+      </c>
+      <c r="C164" s="8"/>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" s="8">
+        <v>164</v>
+      </c>
+      <c r="C165" s="8"/>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" s="8">
+        <v>165</v>
+      </c>
+      <c r="C166" s="8"/>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" s="8">
+        <v>166</v>
+      </c>
+      <c r="C167" s="8"/>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" s="8">
+        <v>167</v>
+      </c>
+      <c r="C168" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D168" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" s="8">
+        <v>168</v>
+      </c>
+      <c r="C169" s="8"/>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" s="8">
+        <v>169</v>
+      </c>
+      <c r="C170" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D170" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" s="8">
+        <v>170</v>
+      </c>
+      <c r="C171" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D171" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" s="8">
+        <v>171</v>
+      </c>
+      <c r="C172" s="8"/>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" s="8">
+        <v>172</v>
+      </c>
+      <c r="C173" s="8"/>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" s="8">
+        <v>173</v>
+      </c>
+      <c r="C174" s="8"/>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" s="8">
+        <v>174</v>
+      </c>
+      <c r="C175" s="8"/>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" s="8">
+        <v>175</v>
+      </c>
+      <c r="C176" s="8"/>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" s="8">
+        <v>176</v>
+      </c>
+      <c r="C177" s="8"/>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178" s="8">
+        <v>177</v>
+      </c>
+      <c r="C178" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D178" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" s="8">
+        <v>178</v>
+      </c>
+      <c r="C179" s="8"/>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" s="8">
+        <v>179</v>
+      </c>
+      <c r="C180" s="8"/>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181" s="8">
+        <v>180</v>
+      </c>
+      <c r="C181" s="8"/>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182" s="8">
+        <v>181</v>
+      </c>
+      <c r="C182" s="8"/>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183" s="8">
+        <v>182</v>
+      </c>
+      <c r="C183" s="8"/>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184" s="8">
+        <v>183</v>
+      </c>
+      <c r="C184" s="8"/>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="A185" s="8">
+        <v>184</v>
+      </c>
+      <c r="C185" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D185" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186" s="8">
+        <v>185</v>
+      </c>
+      <c r="C186" s="8"/>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="A187" s="8">
+        <v>186</v>
+      </c>
+      <c r="C187" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D187" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188" s="8">
+        <v>187</v>
+      </c>
+      <c r="C188" s="8"/>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" s="8">
+        <v>188</v>
+      </c>
+      <c r="C189" s="8"/>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="A190" s="8">
+        <v>189</v>
+      </c>
+      <c r="C190" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D190" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="A191" s="8">
+        <v>190</v>
+      </c>
+      <c r="C191" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D191" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="A192" s="8">
+        <v>191</v>
+      </c>
+      <c r="C192" s="8"/>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="A193" s="8">
+        <v>192</v>
+      </c>
+      <c r="C193" s="8"/>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194" s="8">
+        <v>193</v>
+      </c>
+      <c r="C194" s="8"/>
+    </row>
+    <row r="195" spans="1:4">
+      <c r="A195" s="8">
+        <v>194</v>
+      </c>
+      <c r="C195" s="8"/>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" s="8">
+        <v>195</v>
+      </c>
+      <c r="C196" s="8"/>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" s="8">
+        <v>196</v>
+      </c>
+      <c r="C197" s="8"/>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" s="8">
+        <v>197</v>
+      </c>
+      <c r="C198" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D198" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" s="8">
+        <v>198</v>
+      </c>
+      <c r="C199" s="8"/>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" s="8">
+        <v>199</v>
+      </c>
+      <c r="C200" s="8"/>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201" s="8">
+        <v>200</v>
+      </c>
+      <c r="C201" s="8"/>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C67 C70 C72:C201" xr:uid="{635B544C-31D1-4B3A-889A-7EB2C936CCFC}">
+      <formula1>"English,Knowledge Gaps,Emotion,Techniques"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F1" location="'Domain-Planning'!A1" display="Domain" xr:uid="{5427A910-0EA1-49AD-9406-1920763AE554}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C417280C-3257-4FCE-BFBC-576DD1B4382F}">
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1"/>

</xml_diff>

<commit_message>
phai do phai do
</commit_message>
<xml_diff>
--- a/10_Management/Exam_PMP_Finish_07032019 - TrungLV_Final.xlsx
+++ b/10_Management/Exam_PMP_Finish_07032019 - TrungLV_Final.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Working\EBill\10_Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\EBill\10_Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AB2271-FD1E-41E7-9E9B-01C3FBB2AC70}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB19442-E83A-4A81-B704-3925ACCF1338}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="21" activeTab="26" xr2:uid="{957D22A2-4D54-4148-9DDE-7A2AF7FA87D7}"/>
   </bookViews>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2740" uniqueCount="1405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2742" uniqueCount="1406">
   <si>
     <t>No</t>
   </si>
@@ -4551,6 +4551,9 @@
 - potential risk response - được confirmed ở plan risk response process
 Risk register được get detail và detail through other process trong risk.
 perform qualitative risk analysis là xác định độ ưu tiên individual project risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">risk rating matrix được phát triển bởi công ty để đánh giá risk chính vì thế nó cần được chuẩn bóa (standardized) và không được thay đổi vì sẽ khiến khó đánh giá sự khác nhau giữa các dự án =&gt; ma trận đánh giá rủi ro: risk rating matrix </t>
   </si>
 </sst>
 </file>
@@ -40121,8 +40124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B257369-A694-4BAC-BC83-9F2B4219DD5E}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40161,13 +40164,17 @@
       </c>
       <c r="E2" s="15"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="75">
       <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="C3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>1405</v>
+      </c>
       <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:6">
@@ -55561,12 +55568,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="B5:K5"/>
     <mergeCell ref="B13:K13"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="B8:K8"/>
@@ -55574,6 +55575,12 @@
     <mergeCell ref="B10:K10"/>
     <mergeCell ref="B11:K11"/>
     <mergeCell ref="B12:K12"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>